<commit_message>
React JS Practice Start
Created First  File
</commit_message>
<xml_diff>
--- a/Attendance JS after Eid.xlsx
+++ b/Attendance JS after Eid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WEB Community\JavaScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BD122A-EFE3-474F-86E5-70CA5C3DE235}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13788F42-A66F-48BC-91A6-5E684BF298E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1725" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
   <si>
     <t>NAME</t>
   </si>
@@ -1032,6 +1032,15 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="27" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="42" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1055,15 +1064,6 @@
     </xf>
     <xf numFmtId="0" fontId="41" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="27" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="27" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1539,8 +1539,8 @@
   </sheetPr>
   <dimension ref="A1:AO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL14" sqref="AL14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1623,42 +1623,42 @@
       <c r="A2" s="33"/>
       <c r="B2" s="33"/>
       <c r="C2" s="33"/>
-      <c r="D2" s="55" t="s">
+      <c r="D2" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="55"/>
-      <c r="AF2" s="55"/>
-      <c r="AG2" s="55"/>
-      <c r="AH2" s="55"/>
-      <c r="AI2" s="55"/>
-      <c r="AJ2" s="55"/>
-      <c r="AK2" s="55"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="58"/>
+      <c r="AC2" s="58"/>
+      <c r="AD2" s="58"/>
+      <c r="AE2" s="58"/>
+      <c r="AF2" s="58"/>
+      <c r="AG2" s="58"/>
+      <c r="AH2" s="58"/>
+      <c r="AI2" s="58"/>
+      <c r="AJ2" s="58"/>
+      <c r="AK2" s="58"/>
       <c r="AL2" s="34"/>
       <c r="AM2" s="5"/>
       <c r="AN2" s="5"/>
@@ -1709,42 +1709,42 @@
       <c r="A4" s="33"/>
       <c r="B4" s="33"/>
       <c r="C4" s="33"/>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
-      <c r="X4" s="56"/>
-      <c r="Y4" s="56"/>
-      <c r="Z4" s="56"/>
-      <c r="AA4" s="56"/>
-      <c r="AB4" s="56"/>
-      <c r="AC4" s="56"/>
-      <c r="AD4" s="56"/>
-      <c r="AE4" s="56"/>
-      <c r="AF4" s="56"/>
-      <c r="AG4" s="56"/>
-      <c r="AH4" s="56"/>
-      <c r="AI4" s="56"/>
-      <c r="AJ4" s="56"/>
-      <c r="AK4" s="56"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="59"/>
+      <c r="AA4" s="59"/>
+      <c r="AB4" s="59"/>
+      <c r="AC4" s="59"/>
+      <c r="AD4" s="59"/>
+      <c r="AE4" s="59"/>
+      <c r="AF4" s="59"/>
+      <c r="AG4" s="59"/>
+      <c r="AH4" s="59"/>
+      <c r="AI4" s="59"/>
+      <c r="AJ4" s="59"/>
+      <c r="AK4" s="59"/>
       <c r="AL4" s="34"/>
       <c r="AM4" s="11"/>
     </row>
@@ -1792,10 +1792,10 @@
       <c r="A6" s="33"/>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="50"/>
+      <c r="E6" s="53"/>
       <c r="F6" s="27" t="s">
         <v>37</v>
       </c>
@@ -1829,7 +1829,7 @@
       <c r="P6" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="Q6" s="53" t="s">
+      <c r="Q6" s="56" t="s">
         <v>38</v>
       </c>
       <c r="R6" s="34"/>
@@ -1863,8 +1863,8 @@
       <c r="A7" s="33"/>
       <c r="B7" s="33"/>
       <c r="C7" s="33"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="52"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55"/>
       <c r="F7" s="9">
         <v>25</v>
       </c>
@@ -1880,13 +1880,15 @@
       <c r="J7" s="9">
         <v>29</v>
       </c>
-      <c r="K7" s="9"/>
+      <c r="K7" s="9">
+        <v>30</v>
+      </c>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9"/>
-      <c r="Q7" s="54"/>
+      <c r="Q7" s="57"/>
       <c r="R7" s="34"/>
       <c r="S7" s="34"/>
       <c r="T7" s="34"/>
@@ -1934,15 +1936,17 @@
       <c r="J8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K8" s="10"/>
+      <c r="K8" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
       <c r="O8" s="10"/>
       <c r="P8" s="10"/>
       <c r="Q8" s="29">
-        <f>COUNTA(F8:P8)</f>
-        <v>3</v>
+        <f t="shared" ref="Q8:Q21" si="1">COUNTA(F8:P8)</f>
+        <v>4</v>
       </c>
       <c r="R8" s="38"/>
       <c r="S8" s="39" t="s">
@@ -1976,22 +1980,22 @@
         <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
-      <c r="E9" s="58" t="s">
+      <c r="E9" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="57"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="57"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="49"/>
       <c r="P9" s="10"/>
       <c r="Q9" s="29">
-        <f>COUNTA(F9:P9)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R9" s="38"/>
@@ -2024,22 +2028,22 @@
         <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="49"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="29">
-        <f>COUNTA(F10:P10)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R10" s="38"/>
@@ -2101,7 +2105,7 @@
       <c r="O11" s="10"/>
       <c r="P11" s="10"/>
       <c r="Q11" s="29">
-        <f>COUNTA(F11:P11)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R11" s="38"/>
@@ -2139,19 +2143,19 @@
       <c r="E12" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="57"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
+      <c r="M12" s="49"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="29">
-        <f>COUNTA(F12:P12)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R12" s="38"/>
@@ -2202,15 +2206,17 @@
       <c r="J13" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="10"/>
+      <c r="K13" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="29">
-        <f>COUNTA(F13:P13)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="R13" s="38"/>
       <c r="S13" s="37" t="s">
@@ -2258,15 +2264,17 @@
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
+      <c r="K14" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="29">
-        <f>COUNTA(F14:P14)</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="R14" s="38"/>
       <c r="S14" s="37" t="s">
@@ -2325,7 +2333,7 @@
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="29">
-        <f>COUNTA(F15:P15)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="R15" s="38"/>
@@ -2378,15 +2386,17 @@
       <c r="J16" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K16" s="10"/>
+      <c r="K16" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
       <c r="Q16" s="29">
-        <f>COUNTA(F16:P16)</f>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="R16" s="38"/>
       <c r="S16" s="40"/>
@@ -2434,15 +2444,17 @@
       <c r="J17" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="10"/>
+      <c r="K17" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
       <c r="Q17" s="29">
-        <f>COUNTA(F17:P17)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="R17" s="38"/>
       <c r="S17" s="34"/>
@@ -2490,15 +2502,17 @@
       <c r="J18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K18" s="10"/>
+      <c r="K18" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
       <c r="Q18" s="29">
-        <f>COUNTA(F18:P18)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="R18" s="38"/>
       <c r="S18" s="34"/>
@@ -2546,15 +2560,17 @@
       <c r="J19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="K19" s="10"/>
+      <c r="K19" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>
       <c r="Q19" s="29">
-        <f>COUNTA(F19:P19)</f>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="R19" s="38"/>
       <c r="S19" s="34"/>
@@ -2585,22 +2601,22 @@
       <c r="D20" s="46">
         <v>13</v>
       </c>
-      <c r="E20" s="58" t="s">
+      <c r="E20" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="F20" s="57"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="57"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-      <c r="O20" s="57"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
+      <c r="O20" s="49"/>
       <c r="P20" s="10"/>
       <c r="Q20" s="29">
-        <f>COUNTA(F20:P20)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R20" s="38"/>
@@ -2633,22 +2649,22 @@
         <f t="shared" ca="1" si="0"/>
         <v>14</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E21" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F21" s="57"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="57"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="57"/>
-      <c r="K21" s="57"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="57"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="57"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="49"/>
+      <c r="O21" s="49"/>
       <c r="P21" s="10"/>
       <c r="Q21" s="29">
-        <f>COUNTA(F21:P21)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R21" s="38"/>
@@ -2682,23 +2698,23 @@
         <v>1</v>
       </c>
       <c r="F22" s="30">
-        <f t="shared" ref="F22:P22" si="1">COUNTA(F8:F21)</f>
+        <f t="shared" ref="F22:P22" si="2">COUNTA(F8:F21)</f>
         <v>7</v>
       </c>
       <c r="G22" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="H22" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="I22" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="J22" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="K22" s="30"/>
@@ -2707,7 +2723,7 @@
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
       <c r="P22" s="30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q22" s="45"/>

</xml_diff>